<commit_message>
fixing assay dict output to confirm function in DS, adding new assays to templates, correct string testing, dropping trailing protocol irrelevant to templating engine as well as input sample nodes defined by mtbls:->to do check with metalights
</commit_message>
<xml_diff>
--- a/isatools/net/resources/mtbls/StudyTerms4Curators-template.xlsx
+++ b/isatools/net/resources/mtbls/StudyTerms4Curators-template.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippe/Documents/git/isa-api2/isa-api/isatools/net/resources/mtbls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945C51FA-C766-7E4D-803B-46D875ACBFE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899FA1AC-47C1-1D46-8ED5-8FA36966E5B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{706403F5-489F-AD48-8BF2-F3744C7F4E3A}"/>
+    <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{706403F5-489F-AD48-8BF2-F3744C7F4E3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="GC-MS Study" sheetId="1" r:id="rId1"/>
-    <sheet name="LC-MS Study" sheetId="2" r:id="rId2"/>
-    <sheet name="NMR Study" sheetId="3" r:id="rId3"/>
+    <sheet name="NMR Study" sheetId="3" r:id="rId1"/>
+    <sheet name="GC-MS Study" sheetId="1" r:id="rId2"/>
+    <sheet name="Imaging-MS Study" sheetId="11" r:id="rId3"/>
+    <sheet name="LC-MS Study" sheetId="2" r:id="rId4"/>
+    <sheet name="CE-MS Study" sheetId="6" r:id="rId5"/>
+    <sheet name="MALDI-MS Study" sheetId="7" r:id="rId6"/>
+    <sheet name="SPE-IMS-MS Study" sheetId="8" r:id="rId7"/>
+    <sheet name="FIA-MS Study" sheetId="5" r:id="rId8"/>
+    <sheet name="DI-MS Study" sheetId="4" r:id="rId9"/>
+    <sheet name="GCxGC-MS Study" sheetId="9" r:id="rId10"/>
+    <sheet name="LC-DAD Study" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="550">
   <si>
     <t>Parameter Value[Chromatography Instrument]</t>
   </si>
@@ -1494,6 +1502,189 @@
   </si>
   <si>
     <t>Parameter Value[NMR Pulse Sequence Name]</t>
+  </si>
+  <si>
+    <t>Agilent 1100 Series Isocratic Pump, G1603A CE-MS Adapter Kit, and G1607A CE-ESI-MS Sprayer Kit</t>
+  </si>
+  <si>
+    <t>CE bare fused-silica capillary (50 μm x 800 mm; Agilent Technologies)</t>
+  </si>
+  <si>
+    <t>Agilent 1600A Capillary Electrophoresis, Agilent 1100 Series Isocratic Pump, and G1607A CE-ESI-MS Sprayer Kit</t>
+  </si>
+  <si>
+    <t>CE bare fused-silica capillary (50 μm x 1,000 mm; Agilent Technologies)</t>
+  </si>
+  <si>
+    <t>Agilent 7100 CE System</t>
+  </si>
+  <si>
+    <t>Parameter Value[Cartridge type]</t>
+  </si>
+  <si>
+    <t>Agilent RapidFire 365</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>mixed mode</t>
+  </si>
+  <si>
+    <t>graphitic carbon</t>
+  </si>
+  <si>
+    <t>Parameter Value[Detector]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Signal range]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Resolution]</t>
+  </si>
+  <si>
+    <t>Waters ACQUITY UPLC PDA Detector</t>
+  </si>
+  <si>
+    <t>190-500 nm</t>
+  </si>
+  <si>
+    <t>0.25 nm</t>
+  </si>
+  <si>
+    <t>210-450 nm</t>
+  </si>
+  <si>
+    <t>2 nm</t>
+  </si>
+  <si>
+    <t>Waters ACQUITY UPLC PDA eλ Detector</t>
+  </si>
+  <si>
+    <t>250-600 nm</t>
+  </si>
+  <si>
+    <t>1.2 nm</t>
+  </si>
+  <si>
+    <t>Agilent 1290 Infinity DAD Detector</t>
+  </si>
+  <si>
+    <t>200-600 nm</t>
+  </si>
+  <si>
+    <t>1 nm</t>
+  </si>
+  <si>
+    <t>Parameter Value[Instrument]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Ion source]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Mass analyzer]</t>
+  </si>
+  <si>
+    <t>AB SCIEX 4800 Plus MALDI TOF/TOF</t>
+  </si>
+  <si>
+    <t>MS:matrix-assisted laser desorption ionization</t>
+  </si>
+  <si>
+    <t>MS:time-of-flight</t>
+  </si>
+  <si>
+    <t>AB SCIEX TOF/TOF 5800</t>
+  </si>
+  <si>
+    <t>Bruker ultrafleXtreme</t>
+  </si>
+  <si>
+    <t>Parameter Value[Sample mounting]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Sample preservation]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Sectioning instrument]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Line scan direction]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Line scan sequence]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Scan pattern]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Scan type]</t>
+  </si>
+  <si>
+    <t>Glass slide</t>
+  </si>
+  <si>
+    <t>Fresh frozen</t>
+  </si>
+  <si>
+    <t>Thermo Scientific Shandon Cryotome</t>
+  </si>
+  <si>
+    <t>Bruker solariX XR</t>
+  </si>
+  <si>
+    <t>MS:electrospray ionization</t>
+  </si>
+  <si>
+    <t>Hybrid Qh-FTMS</t>
+  </si>
+  <si>
+    <t>linescan left right</t>
+  </si>
+  <si>
+    <t>top down</t>
+  </si>
+  <si>
+    <t>flyback</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>Thermo Scientific X72 SuperFrost Plus Adhesion slide</t>
+  </si>
+  <si>
+    <t>Thermo Scientific Microm HM550 Cryostat</t>
+  </si>
+  <si>
+    <t>Thermo Scientific LTQ Orbitrap XL ETD</t>
+  </si>
+  <si>
+    <t>MS:orbitrap</t>
+  </si>
+  <si>
+    <t>Thermo Scientific FB58628 Fisherbrand Glass slide</t>
+  </si>
+  <si>
+    <t>Leica CM3050 S</t>
+  </si>
+  <si>
+    <t>Thermo Scientific MALDI LTQ Orbitrap XL</t>
+  </si>
+  <si>
+    <t>Thermo Scientific SuperFrost Glass slide</t>
+  </si>
+  <si>
+    <t>Thermo Scientific MALDI LTQ Orbitrap Discovery</t>
+  </si>
+  <si>
+    <t>Delta Electronics ITO one surface glass slide</t>
+  </si>
+  <si>
+    <t>Thermo Scientific Orbitrap Elite</t>
+  </si>
+  <si>
+    <t>Thermo Scientific Polysine Adhesion Slide</t>
   </si>
 </sst>
 </file>
@@ -1879,1974 +2070,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C254300-16D0-D248-B3F0-2FDF8F57C687}">
-  <dimension ref="A1:C54"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C54"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-      <c r="B41" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-      <c r="B42" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-      <c r="B43" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-      <c r="B49" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
-      <c r="B51" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
-      <c r="B52" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
-      <c r="B53" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
-      <c r="B54" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48467566-1CAC-7F4D-AEFD-016885F11A7F}">
-  <dimension ref="A1:C142"/>
-  <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="77.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="2"/>
-      <c r="B78" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
-      <c r="B79" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="2"/>
-      <c r="B80" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="2"/>
-      <c r="B81" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="2"/>
-      <c r="B82" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="2"/>
-      <c r="B91" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="4"/>
-      <c r="B102" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="4"/>
-      <c r="B114" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="4"/>
-      <c r="B115" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="4"/>
-      <c r="B116" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="4"/>
-      <c r="B118" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="4"/>
-      <c r="B119" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="4"/>
-      <c r="B120" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" s="4"/>
-      <c r="B122" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="4"/>
-      <c r="B123" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="4"/>
-      <c r="B124" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="4"/>
-      <c r="B125" s="4" t="s">
-        <v>467</v>
-      </c>
-      <c r="C125" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="4"/>
-      <c r="B126" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="4"/>
-      <c r="B127" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="4"/>
-      <c r="B128" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" s="4"/>
-      <c r="B129" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="4"/>
-      <c r="B130" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="4"/>
-      <c r="B131" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="4"/>
-      <c r="B132" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="4"/>
-      <c r="B133" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="4"/>
-      <c r="B134" s="4" t="s">
-        <v>476</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="C135" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="4"/>
-      <c r="B136" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="4"/>
-      <c r="B137" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="C137" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="4"/>
-      <c r="B138" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="C138" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A139" s="4"/>
-      <c r="B139" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A140" s="4"/>
-      <c r="B140" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A141" s="4"/>
-      <c r="B141" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C141" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" s="4"/>
-      <c r="B142" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D450F36E-855A-3542-AFDF-1AFE50D8F16E}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -5163,4 +3390,2405 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABE336B-C957-A24B-91FC-40EFB372645A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CBCE48-FCF0-4B47-BBDB-1E6AE2D65D2B}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C254300-16D0-D248-B3F0-2FDF8F57C687}">
+  <dimension ref="A1:C54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2B4E28-BE4D-0948-97DA-16FE864AE229}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48467566-1CAC-7F4D-AEFD-016885F11A7F}">
+  <dimension ref="A1:C142"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="77.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="2"/>
+      <c r="B78" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="2"/>
+      <c r="B79" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="2"/>
+      <c r="B80" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="2"/>
+      <c r="B81" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="2"/>
+      <c r="B82" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="2"/>
+      <c r="B91" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="4"/>
+      <c r="B136" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="4"/>
+      <c r="B137" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222840EC-7592-7D48-AA3B-7D7A0EF590D0}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C14FF2-CC79-D442-B0E6-422E62A14C02}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C632FBF-2E0D-334A-97F1-E292FC3C4994}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EE4EB0-54A7-2A4B-BCAD-3664F7E17E03}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54972E6D-43D6-7748-98EB-76A958077041}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>